<commit_message>
kröfulisti með c kröfu
</commit_message>
<xml_diff>
--- a/krofulisti.xlsx
+++ b/krofulisti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gudmundur\Dropbox\Tölvunarfræði\Verk1\hópverk\verklegtnamskeid1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5839C28C-E44C-495E-8511-09C3E6655AF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2ABE1C-2AA3-494F-ABDC-10CD3568EEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16032" yWindow="3732" windowWidth="23256" windowHeight="12576" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="kröfur" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="53">
   <si>
     <t>Number</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Það þarf að vera hægt að sjá lista yfir stöðu allra flugvélanna miðað við ákveðna dagsetningu og tíma ásamt nafni, týpu og sætafjölda</t>
   </si>
   <si>
-    <t>allir</t>
-  </si>
-  <si>
     <t>Það þarf að vera hægt að sjá stöðu vinnuferðar miðað við núverandi dagsetningu og tíma. Mögulegar stöður:  lokið, lent ytra, í loftinu, ekki hafin</t>
   </si>
   <si>
@@ -185,6 +182,15 @@
   </si>
   <si>
     <t>Það þarf að vera hægt að sjá lista yfir allar vinnuferðir í ákveðinni viku  og gefa til kynna hvort þær séu fullmannaðar eða ekki</t>
+  </si>
+  <si>
+    <t>Það þarf að vera hægt að sjá lista yfir allar flugvélategund og hve margir flugmenn hafa réttindi á viðkomandi tegund</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Allir</t>
   </si>
 </sst>
 </file>
@@ -729,20 +735,20 @@
   </sheetPr>
   <dimension ref="B2:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C32" zoomScale="127" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="59.44140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="59.453125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
@@ -759,16 +765,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="20"/>
       <c r="C3" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
       <c r="F3" s="24"/>
     </row>
-    <row r="4" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="14">
         <v>1</v>
       </c>
@@ -783,7 +789,7 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B5" s="6">
         <v>2</v>
       </c>
@@ -798,7 +804,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B6" s="14">
         <v>3</v>
       </c>
@@ -813,7 +819,7 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="6">
         <v>4</v>
       </c>
@@ -828,7 +834,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="14">
         <v>5</v>
       </c>
@@ -843,7 +849,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B9" s="6">
         <v>6</v>
       </c>
@@ -858,7 +864,7 @@
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="14">
         <v>7</v>
       </c>
@@ -873,7 +879,7 @@
       </c>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="6">
         <v>8</v>
       </c>
@@ -888,7 +894,7 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="14">
         <v>9</v>
       </c>
@@ -903,7 +909,7 @@
       </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="6">
         <v>10</v>
       </c>
@@ -918,7 +924,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="14">
         <v>11</v>
       </c>
@@ -933,7 +939,7 @@
       </c>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="6">
         <v>12</v>
       </c>
@@ -941,14 +947,14 @@
         <v>19</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="14">
         <v>13</v>
       </c>
@@ -956,19 +962,19 @@
         <v>20</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>8</v>
@@ -978,7 +984,7 @@
       </c>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="2:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="22.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="14">
         <v>15</v>
       </c>
@@ -993,7 +999,7 @@
       </c>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
         <v>16</v>
       </c>
@@ -1008,7 +1014,7 @@
       </c>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B20" s="14">
         <v>17</v>
       </c>
@@ -1023,12 +1029,12 @@
       </c>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="6">
         <v>18</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>8</v>
@@ -1038,7 +1044,7 @@
       </c>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="14">
         <v>19</v>
       </c>
@@ -1053,7 +1059,7 @@
       </c>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="6">
         <v>20</v>
       </c>
@@ -1068,7 +1074,7 @@
       </c>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B24" s="14">
         <v>21</v>
       </c>
@@ -1083,7 +1089,7 @@
       </c>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="6">
         <v>22</v>
       </c>
@@ -1098,7 +1104,7 @@
       </c>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6">
         <v>23</v>
       </c>
@@ -1113,7 +1119,7 @@
       </c>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B27" s="6">
         <v>24</v>
       </c>
@@ -1128,12 +1134,12 @@
       </c>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B28" s="6">
         <v>25</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>8</v>
@@ -1143,7 +1149,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B29" s="6">
         <v>26</v>
       </c>
@@ -1158,12 +1164,12 @@
       </c>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="6">
         <v>27</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>8</v>
@@ -1173,7 +1179,7 @@
       </c>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B31" s="6">
         <v>28</v>
       </c>
@@ -1188,12 +1194,12 @@
       </c>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B32" s="6">
         <v>29</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>21</v>
@@ -1203,57 +1209,57 @@
       </c>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="6">
         <v>30</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="11"/>
     </row>
-    <row r="34" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="6">
         <v>31</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F34" s="11"/>
     </row>
-    <row r="35" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B35" s="6">
         <v>32</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F35" s="19"/>
     </row>
-    <row r="36" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="6">
         <v>33</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>21</v>
@@ -1263,7 +1269,7 @@
       </c>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="6">
         <v>34</v>
       </c>
@@ -1271,14 +1277,14 @@
         <v>39</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="6">
         <v>35</v>
       </c>
@@ -1286,14 +1292,14 @@
         <v>36</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F38" s="11"/>
     </row>
-    <row r="39" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B39" s="6">
         <v>36</v>
       </c>
@@ -1301,14 +1307,14 @@
         <v>37</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F39" s="11"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B40" s="6">
         <v>37</v>
       </c>
@@ -1316,20 +1322,26 @@
         <v>38</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F40" s="11"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B41" s="6">
         <v>38</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="5"/>
+      <c r="C41" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="F41" s="11"/>
     </row>
   </sheetData>
@@ -1346,14 +1358,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Fixed wording and completed the first draft of use cases
</commit_message>
<xml_diff>
--- a/krofulisti.xlsx
+++ b/krofulisti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gudmundur\Dropbox\Tölvunarfræði\Verk1\hópverk\verklegtnamskeid1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\runar\Desktop\verklegtnamskeid1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2ABE1C-2AA3-494F-ABDC-10CD3568EEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF69DE07-7C73-4F88-9630-EDAC2B0B224E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4B1D200-2CAD-450F-B296-0F19F81F2DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="kröfur" sheetId="2" r:id="rId1"/>
@@ -136,9 +136,6 @@
     <t>Það þarf að vera hægt að skrá flugvél á vinnuferð áður en starfsmenn eru skráðir</t>
   </si>
   <si>
-    <t>Það þarf að vera hægt að skrá tvö flugnúmer á vinnuferð þar sem fyrrihluti númeranna samanstendur af einkenni áfangastaðar og seinni hluti eftir fjölda ferða þess dags þar sem talan skal vera næsta slétta tala ef farið er frá Íslandi en næsta oddatala ef farið er til íslands</t>
-  </si>
-  <si>
     <t>Það þarf að vera hægt að skrá áfangastað með landi, flugvelli, einkennisnúmer flugvallar, flugtíma og fjarlægð frá Íslandi ásamt nafni tengiliðs og neyðarsímanúmeri</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>Það þarf að vera hægt að sjá lista yfir alla vinnuferðir með fjölda lausra- og seldra sæta</t>
   </si>
   <si>
-    <t>Það þarf að að hægt að breyta nafni á tengiliði og/eða neyðarsímanúmeri sem skráð er fyrir áfangastað</t>
-  </si>
-  <si>
     <t>Það þarf að vera hægt að sjá lista yfir alla vinnuferðir með flugnúmerum beggja flugferðanna</t>
   </si>
   <si>
@@ -184,13 +178,19 @@
     <t>Það þarf að vera hægt að sjá lista yfir allar vinnuferðir í ákveðinni viku  og gefa til kynna hvort þær séu fullmannaðar eða ekki</t>
   </si>
   <si>
-    <t>Það þarf að vera hægt að sjá lista yfir allar flugvélategund og hve margir flugmenn hafa réttindi á viðkomandi tegund</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
     <t>Allir</t>
+  </si>
+  <si>
+    <t>Það þarf að vera hægt að sjá lista yfir allar flugvélategundir og hve margir flugmenn hafa réttindi á viðkomandi tegund</t>
+  </si>
+  <si>
+    <t>Það þarf að hægt að breyta nafni á tengiliði og/eða neyðarsímanúmeri sem skráð er fyrir áfangastað</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Það þarf að vera hægt að skrá tvö flugnúmer á vinnuferð </t>
   </si>
 </sst>
 </file>
@@ -735,20 +735,20 @@
   </sheetPr>
   <dimension ref="B2:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.90625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="59.453125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
@@ -765,16 +765,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="20"/>
       <c r="C3" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="23"/>
       <c r="F3" s="24"/>
     </row>
-    <row r="4" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="14">
         <v>1</v>
       </c>
@@ -789,12 +789,12 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>21</v>
@@ -804,7 +804,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>3</v>
       </c>
@@ -819,7 +819,7 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
         <v>4</v>
       </c>
@@ -834,7 +834,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="14">
         <v>5</v>
       </c>
@@ -849,7 +849,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
         <v>6</v>
       </c>
@@ -864,7 +864,7 @@
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="14">
         <v>7</v>
       </c>
@@ -879,7 +879,7 @@
       </c>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="6">
         <v>8</v>
       </c>
@@ -894,7 +894,7 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="14">
         <v>9</v>
       </c>
@@ -909,7 +909,7 @@
       </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="6">
         <v>10</v>
       </c>
@@ -924,7 +924,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="14">
         <v>11</v>
       </c>
@@ -939,7 +939,7 @@
       </c>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <v>12</v>
       </c>
@@ -947,14 +947,14 @@
         <v>19</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="14">
         <v>13</v>
       </c>
@@ -962,19 +962,19 @@
         <v>20</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="6">
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>8</v>
@@ -984,7 +984,7 @@
       </c>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="2:6" ht="22.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14">
         <v>15</v>
       </c>
@@ -999,7 +999,7 @@
       </c>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
         <v>16</v>
       </c>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="14">
         <v>17</v>
       </c>
@@ -1029,12 +1029,12 @@
       </c>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
         <v>18</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>8</v>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="14">
         <v>19</v>
       </c>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="6">
         <v>20</v>
       </c>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="14">
         <v>21</v>
       </c>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="6">
         <v>22</v>
       </c>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6">
         <v>23</v>
       </c>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="6">
         <v>24</v>
       </c>
@@ -1134,12 +1134,12 @@
       </c>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" s="6">
         <v>25</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>8</v>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="F28" s="11"/>
     </row>
-    <row r="29" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="6">
         <v>26</v>
       </c>
@@ -1164,12 +1164,12 @@
       </c>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B30" s="6">
         <v>27</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>8</v>
@@ -1179,12 +1179,12 @@
       </c>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="6">
         <v>28</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>21</v>
@@ -1194,12 +1194,12 @@
       </c>
       <c r="F31" s="11"/>
     </row>
-    <row r="32" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B32" s="6">
         <v>29</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>21</v>
@@ -1209,57 +1209,57 @@
       </c>
       <c r="F32" s="11"/>
     </row>
-    <row r="33" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="6">
         <v>30</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="11"/>
     </row>
-    <row r="34" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B34" s="6">
         <v>31</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F34" s="11"/>
     </row>
-    <row r="35" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B35" s="6">
         <v>32</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F35" s="19"/>
     </row>
-    <row r="36" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B36" s="6">
         <v>33</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>21</v>
@@ -1269,67 +1269,67 @@
       </c>
       <c r="F36" s="11"/>
     </row>
-    <row r="37" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="6">
         <v>34</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F37" s="11"/>
     </row>
-    <row r="38" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B38" s="6">
         <v>35</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F38" s="11"/>
     </row>
-    <row r="39" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B39" s="6">
         <v>36</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F39" s="11"/>
     </row>
-    <row r="40" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="6">
         <v>37</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F40" s="11"/>
     </row>
-    <row r="41" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B41" s="6">
         <v>38</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>8</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F41" s="11"/>
     </row>
@@ -1358,14 +1358,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>7</v>
       </c>

</xml_diff>